<commit_message>
fix: typo in blog post
</commit_message>
<xml_diff>
--- a/content/post/2023-web-scraping/ordinary_serums.xlsx
+++ b/content/post/2023-web-scraping/ordinary_serums.xlsx
@@ -104,7 +104,7 @@
     <t xml:space="preserve">6 months after opening.</t>
   </si>
   <si>
-    <t xml:space="preserve">with Direct Acids Direct Vitamin C Resveratrol and Ferulic Acid Salicylic Acid EUK Retinoids Strong Antioxidants</t>
+    <t xml:space="preserve">with Direct Acids Direct Vitamin C EUK Retinoids Strong Antioxidants Resveratrol and Ferulic Acid Salicylic Acid</t>
   </si>
   <si>
     <t xml:space="preserve">The Ordinary Argireline Solution 10%</t>
@@ -122,6 +122,30 @@
     <t xml:space="preserve">The Multi-Peptide Lash and Brow Serum is a light, non-greasy formula designed to support thicker, fuller, and healthier-looking lashes and brows. By utilizing 11 active ingredients, including four peptide complexes and a series of natural extracts, this twice-daily serum works to help nourish and protect your lashes and brows while enhancing the look of density and overall appearance in as little as four weeks.This formula contains SYMPEPTIDE XLASH® complex (with Myristoyl Pentapeptide-17), Anargy® complex (with Oligopeptide-2 and Glycoproteins), Widelash™ complex (with Biotinoyl Tripeptide-1 and Panthenol), REDENSYL™ complex (with Larix Europaea Wood Extract, Camellia Sinensis Leaf Extract, and Zinc Chloride), CAPIXYL™ complex (Acetyl Tetrapeptide-3 and Trifolium Pratense Flower Extract), and High-Solubility Caffeine.All trademarks belong to their respective owners. SYMPEPTIDE XLASH® is a registered trademark of SYMRISE AG, Anargy® is a registered trademark of LIPOTRUE, S.L., Widelash™ is a trademark of Sederma Inc., REDENSYL™ is a trademark of Givaudan, and CAPIXYL™ is a trademark of Lucas Meyer Cosmetics Canada Inc. Neither DECIEM nor The Ordinary is affiliated with the trademark owners. </t>
   </si>
   <si>
+    <t xml:space="preserve">The Ordinary Granactive Retinoid 5% in Squalane</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Textural Irregularities, Signs of Aging, Uneven Skin Tone</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dry Skin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Anhydrous Serum</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Granactive Retinoid 5% in Squalane is a light, oil-like serum that targets visible signs of aging through a highly-advanced retinoid active, one of the best all-around ingredients for skin. This next-generation retinoid improves the appearance of fine and dynamic lines that arise from a loss of collagen and elastin while evening skin texture and tone. It’s further supported with squalane, a moisturizing agent naturally found in the skin. That means it not only delivers comparable visible results to retinol, it’s less likely to cause irritation.Granactive Retinoid™ is a trademark of Grant Industries. Neither DECIEM nor The Ordinary is affiliated with Grant Industries.Note: Once opened, this formula should be refrigerated and used within a three-month period.Caution: Retinoids can make the skin more sensitive to UV radiation. Sun protection is particularly important when using retinoids. This product must not be used in conjunction with other retinoids including retinol or retinoic acid. This product is not a treatment for acne.Note: When pregnant or breastfeeding, it is recommended to avoid any skincare products containing retinoids such as formulations with Granactive Retinoid or Retinol.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Use in PM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3 months after opening.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">with Copper Peptides Direct Acids Direct Vitamin C Retinoids</t>
+  </si>
+  <si>
     <t xml:space="preserve">The Ordinary Marine Hyaluronics</t>
   </si>
   <si>
@@ -143,28 +167,13 @@
     <t xml:space="preserve">with Copper Peptides Direct Acids Direct Vitamin C EUK Niacinamide Powder Peptides Retinoids</t>
   </si>
   <si>
-    <t xml:space="preserve">The Ordinary Granactive Retinoid 5% in Squalane</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Textural Irregularities, Signs of Aging, Uneven Skin Tone</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dry Skin</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Anhydrous Serum</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Granactive Retinoid 5% in Squalane is a light, oil-like serum that targets visible signs of aging through a highly-advanced retinoid active, one of the best all-around ingredients for skin. This next-generation retinoid improves the appearance of fine and dynamic lines that arise from a loss of collagen and elastin while evening skin texture and tone. It’s further supported with squalane, a moisturizing agent naturally found in the skin. That means it not only delivers comparable visible results to retinol, it’s less likely to cause irritation.Granactive Retinoid™ is a trademark of Grant Industries. Neither DECIEM nor The Ordinary is affiliated with Grant Industries.Note: Once opened, this formula should be refrigerated and used within a three-month period.Caution: Retinoids can make the skin more sensitive to UV radiation. Sun protection is particularly important when using retinoids. This product must not be used in conjunction with other retinoids including retinol or retinoic acid. This product is not a treatment for acne.Note: When pregnant or breastfeeding, it is recommended to avoid any skincare products containing retinoids such as formulations with Granactive Retinoid or Retinol.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Use in PM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3 months after opening.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">with Copper Peptides Direct Acids Direct Vitamin C Retinoids</t>
+    <t xml:space="preserve">The Ordinary Granactive Retinoid 2% Emulsion</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Emulsion</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Granactive Retinoid 2% Emulsion is a creamy serum that targets visible signs of aging through a highly-advanced retinoid active, one of the best all-around ingredients for skin. This next-generation retinoid improves the appearance of fine and dynamic lines that arise from a loss of collagen and elastin, while evening skin texture and tone. What’s more, this advanced ingredient is not only proven to deliver comparable visible results to retinol; it’s less likely to cause irritation.Granactive Retinoid™ is a trademark of Grant Industries. Neither DECIEM nor The Ordinary is affiliated with Grant Industries.Note: Once opened, this formula should be refrigerated and used within a three-month period.Caution: Retinoids can make the skin more sensitive to UV radiation. Sun protection is particularly important when using retinoids. This product must not be used in conjunction with other retinoids including retinol or retinoic acid. This product is not a treatment for acne.Note: When pregnant or breastfeeding, it is recommended to avoid any skincare products containing retinoids such as formulations with Granactive Retinoid or Retinol.</t>
   </si>
   <si>
     <t xml:space="preserve">The Ordinary Amino Acids + B5</t>
@@ -173,15 +182,6 @@
     <t xml:space="preserve">Amino Acids + B5 is an ultra-thin serum that works with your skin to support its natural hydration barrier. By including a concentrated 17% (by weight) solution of amino acids and amino acid derivatives that mimic your skin’s natural moisturizing factors, this water-based formula keeps the outer layer of your skin protected and well-hydrated without feeling greasy. Plus, it uses 5% (by weight) pro-vitamin B5 to provide surface and below-surface hydration, giving way to softer, smoother skin.</t>
   </si>
   <si>
-    <t xml:space="preserve">The Ordinary Granactive Retinoid 2% Emulsion</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Emulsion</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Granactive Retinoid 2% Emulsion is a creamy serum that targets visible signs of aging through a highly-advanced retinoid active, one of the best all-around ingredients for skin. This next-generation retinoid improves the appearance of fine and dynamic lines that arise from a loss of collagen and elastin, while evening skin texture and tone. What’s more, this advanced ingredient is not only proven to deliver comparable visible results to retinol; it’s less likely to cause irritation.Granactive Retinoid™ is a trademark of Grant Industries. Neither DECIEM nor The Ordinary is affiliated with Grant Industries.Note: Once opened, this formula should be refrigerated and used within a three-month period.Caution: Retinoids can make the skin more sensitive to UV radiation. Sun protection is particularly important when using retinoids. This product must not be used in conjunction with other retinoids including retinol or retinoic acid. This product is not a treatment for acne.Note: When pregnant or breastfeeding, it is recommended to avoid any skincare products containing retinoids such as formulations with Granactive Retinoid or Retinol.</t>
-  </si>
-  <si>
     <t xml:space="preserve">The Ordinary Retinol 0.5% in Squalane</t>
   </si>
   <si>
@@ -272,6 +272,15 @@
     <t xml:space="preserve">Ascorbic Acid 8% + Alpha Arbutin 2% is made with two of the most well-known brightening agents in skincare. Its water-free formula combines direct vitamin C and a high concentration of alpha arbutin to visibly improve pigmentation and balance uneven skin tone. With advanced antioxidant properties, it protects the skin from the visual effects of damage caused by environmental stressors, helping to maintain a more radiant complexion.Note: Vitamin C and Alpha Arbutin are less stable in formulations that contain water and use of them combined in formulations containing water is highly discouraged. This formulation is a water-free, stable solution, and may feel slightly "oily" for a few seconds after application, despite the fact that it is completely free of oil.</t>
   </si>
   <si>
+    <t xml:space="preserve">The Ordinary Alpha Arbutin 2% + HA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Uneven Skin Tone, Dryness</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Alpha Arbutin 2% + HA is a water-based serum specifically designed to target uneven skin tone and visibly improve pigmentation. It combines a high concentration of purified alpha arbutin, a well-known skin-brightening ingredient, with hyaluronic acid. Purified alpha-arbutin works to target dark spots and uneven skin tone. Meanwhile, hyaluronic acid helps to support product absorption into the skin.Note: Alpha Arbutin is extremely sensitive to degradation in the presence of water if the pH of the formulation is not ideal. The pH of this formula has been shown to be the most suitable pH to minimize degradation of Alpha Arbutin.We are aware of the potential colour changes of our Alpha Arbutin product. This is a natural occurrence, where certain ingredients in the product can change colour when exposed to sunlight or increased temperature. Testing has shown that the efficacy and safety profile of the active ingredient remains stable.</t>
+  </si>
+  <si>
     <t xml:space="preserve">The Ordinary 100% Plant-Derived Squalane</t>
   </si>
   <si>
@@ -285,15 +294,6 @@
   </si>
   <si>
     <t xml:space="preserve">Aloe 2% + NAG 2% Solution is a lightweight soothing serum formulated for blemish-prone skin. It reduces the appearance of post-acne marks through the inclusion of ingredients that target the look and feel of both uneven skin tone and texture, while also helping to reduce the appearance of pores, and strengthening skin barrier.This formulation incorporates aloe barbadensis leaf juice powder for hydration. It also contains N-acetyl glucosamine (NAG), a biotechnology-derived ingredient that has been shown to effectively target the appearance of uneven skin tone. It is further supported by peptide technology palmitoyl pentapeptide-4 which targets the feel of textural irregularities, while offering effective barrier support.Testing ShowsReduces the appearance of post-acne marksReduces the look of skin redness caused by irritationReduces the appearance of poresImproves the appearance of uneven skin tone and the feel of uneven skin textureStrengthens and maintains skin barrier functionBoosts skin hydration*Consumer testing on 31 subjects after using product 2x/day for 8 weeks.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The Ordinary Alpha Arbutin 2% + HA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Uneven Skin Tone, Dryness</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Alpha Arbutin 2% + HA is a water-based serum specifically designed to target uneven skin tone and visibly improve pigmentation. It combines a high concentration of purified alpha arbutin, a well-known skin-brightening ingredient, with hyaluronic acid. Purified alpha-arbutin works to target dark spots and uneven skin tone. Meanwhile, hyaluronic acid helps to support product absorption into the skin.Note: Alpha Arbutin is extremely sensitive to degradation in the presence of water if the pH of the formulation is not ideal. The pH of this formula has been shown to be the most suitable pH to minimize degradation of Alpha Arbutin.We are aware of the potential colour changes of our Alpha Arbutin product. This is a natural occurrence, where certain ingredients in the product can change colour when exposed to sunlight or increased temperature. Testing has shown that the efficacy and safety profile of the active ingredient remains stable.</t>
   </si>
   <si>
     <t xml:space="preserve">The Ordinary EUK 134 0.1%</t>
@@ -901,40 +901,42 @@
         <v>36</v>
       </c>
       <c r="B9" t="s">
-        <v>17</v>
+        <v>37</v>
       </c>
       <c r="C9" t="s">
-        <v>10</v>
+        <v>38</v>
       </c>
       <c r="D9" t="s">
-        <v>11</v>
+        <v>39</v>
       </c>
       <c r="E9" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="F9" t="s">
-        <v>13</v>
+        <v>41</v>
       </c>
       <c r="G9" t="s">
-        <v>14</v>
-      </c>
-      <c r="H9"/>
+        <v>42</v>
+      </c>
+      <c r="H9" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="B10" t="s">
-        <v>39</v>
+        <v>17</v>
       </c>
       <c r="C10" t="s">
         <v>10</v>
       </c>
       <c r="D10" t="s">
-        <v>40</v>
+        <v>11</v>
       </c>
       <c r="E10" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="F10" t="s">
         <v>13</v>
@@ -942,31 +944,29 @@
       <c r="G10" t="s">
         <v>14</v>
       </c>
-      <c r="H10" t="s">
-        <v>42</v>
-      </c>
+      <c r="H10"/>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="B11" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="C11" t="s">
-        <v>45</v>
+        <v>10</v>
       </c>
       <c r="D11" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="E11" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="F11" t="s">
-        <v>48</v>
+        <v>13</v>
       </c>
       <c r="G11" t="s">
-        <v>49</v>
+        <v>14</v>
       </c>
       <c r="H11" t="s">
         <v>50</v>
@@ -977,50 +977,50 @@
         <v>51</v>
       </c>
       <c r="B12" t="s">
-        <v>17</v>
+        <v>37</v>
       </c>
       <c r="C12" t="s">
         <v>10</v>
       </c>
       <c r="D12" t="s">
-        <v>11</v>
+        <v>52</v>
       </c>
       <c r="E12" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="F12" t="s">
-        <v>13</v>
+        <v>41</v>
       </c>
       <c r="G12" t="s">
-        <v>14</v>
-      </c>
-      <c r="H12"/>
+        <v>42</v>
+      </c>
+      <c r="H12" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B13" t="s">
-        <v>44</v>
+        <v>17</v>
       </c>
       <c r="C13" t="s">
         <v>10</v>
       </c>
       <c r="D13" t="s">
-        <v>54</v>
+        <v>11</v>
       </c>
       <c r="E13" t="s">
         <v>55</v>
       </c>
       <c r="F13" t="s">
-        <v>48</v>
+        <v>13</v>
       </c>
       <c r="G13" t="s">
-        <v>49</v>
-      </c>
-      <c r="H13" t="s">
-        <v>50</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="H13"/>
     </row>
     <row r="14">
       <c r="A14" t="s">
@@ -1033,19 +1033,19 @@
         <v>10</v>
       </c>
       <c r="D14" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="E14" t="s">
         <v>58</v>
       </c>
       <c r="F14" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="G14" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="H14" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
     </row>
     <row r="15">
@@ -1059,19 +1059,19 @@
         <v>10</v>
       </c>
       <c r="D15" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="E15" t="s">
         <v>60</v>
       </c>
       <c r="F15" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="G15" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="H15" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
     </row>
     <row r="16">
@@ -1085,19 +1085,19 @@
         <v>10</v>
       </c>
       <c r="D16" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="E16" t="s">
         <v>62</v>
       </c>
       <c r="F16" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="G16" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="H16" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
     </row>
     <row r="17">
@@ -1111,7 +1111,7 @@
         <v>10</v>
       </c>
       <c r="D17" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="E17" t="s">
         <v>65</v>
@@ -1135,13 +1135,13 @@
         <v>10</v>
       </c>
       <c r="D18" t="s">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="E18" t="s">
         <v>68</v>
       </c>
       <c r="F18" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="G18" t="s">
         <v>29</v>
@@ -1187,7 +1187,7 @@
         <v>10</v>
       </c>
       <c r="D20" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="E20" t="s">
         <v>75</v>
@@ -1207,25 +1207,25 @@
         <v>77</v>
       </c>
       <c r="B21" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="C21" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="D21" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="E21" t="s">
         <v>78</v>
       </c>
       <c r="F21" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="G21" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="H21" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
     </row>
     <row r="22">
@@ -1239,7 +1239,7 @@
         <v>10</v>
       </c>
       <c r="D22" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="E22" t="s">
         <v>80</v>
@@ -1265,13 +1265,13 @@
         <v>10</v>
       </c>
       <c r="D23" t="s">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="E23" t="s">
         <v>83</v>
       </c>
       <c r="F23" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="G23" t="s">
         <v>29</v>
@@ -1291,7 +1291,7 @@
         <v>10</v>
       </c>
       <c r="D24" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="E24" t="s">
         <v>85</v>
@@ -1311,37 +1311,37 @@
         <v>86</v>
       </c>
       <c r="B25" t="s">
-        <v>64</v>
+        <v>87</v>
       </c>
       <c r="C25" t="s">
         <v>10</v>
       </c>
       <c r="D25" t="s">
-        <v>46</v>
+        <v>11</v>
       </c>
       <c r="E25" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="F25" t="s">
         <v>13</v>
       </c>
       <c r="G25" t="s">
-        <v>29</v>
+        <v>14</v>
       </c>
       <c r="H25"/>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B26" t="s">
-        <v>89</v>
+        <v>64</v>
       </c>
       <c r="C26" t="s">
-        <v>45</v>
+        <v>10</v>
       </c>
       <c r="D26" t="s">
-        <v>11</v>
+        <v>39</v>
       </c>
       <c r="E26" t="s">
         <v>90</v>
@@ -1350,11 +1350,9 @@
         <v>13</v>
       </c>
       <c r="G26" t="s">
-        <v>14</v>
-      </c>
-      <c r="H26" t="s">
-        <v>22</v>
-      </c>
+        <v>29</v>
+      </c>
+      <c r="H26"/>
     </row>
     <row r="27">
       <c r="A27" t="s">
@@ -1364,7 +1362,7 @@
         <v>92</v>
       </c>
       <c r="C27" t="s">
-        <v>10</v>
+        <v>38</v>
       </c>
       <c r="D27" t="s">
         <v>11</v>
@@ -1378,7 +1376,9 @@
       <c r="G27" t="s">
         <v>14</v>
       </c>
-      <c r="H27"/>
+      <c r="H27" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
@@ -1391,7 +1391,7 @@
         <v>10</v>
       </c>
       <c r="D28" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="E28" t="s">
         <v>95</v>
@@ -1423,7 +1423,7 @@
         <v>99</v>
       </c>
       <c r="F29" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="G29" t="s">
         <v>29</v>
@@ -1443,7 +1443,7 @@
         <v>10</v>
       </c>
       <c r="D30" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="E30" t="s">
         <v>101</v>
@@ -1492,10 +1492,10 @@
         <v>67</v>
       </c>
       <c r="C32" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="D32" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="E32" t="s">
         <v>108</v>

</xml_diff>

<commit_message>
fix: summary of webscraping post (and rerender)
</commit_message>
<xml_diff>
--- a/content/post/2023-web-scraping/ordinary_serums.xlsx
+++ b/content/post/2023-web-scraping/ordinary_serums.xlsx
@@ -38,37 +38,106 @@
     <t xml:space="preserve">do_not_use</t>
   </si>
   <si>
+    <t xml:space="preserve">The Ordinary Hyaluronic Acid 2% + B5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dryness</t>
+  </si>
+  <si>
+    <t xml:space="preserve">All Skin Types</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Water-based Serum</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hyaluronic Acid 2% + B5 is a water-based formula combining low-, medium- and high-molecular-weight hyaluronic acid molecules and a next-generation HA crosspolymer to support hydration to multiple layers of your skin. It also targets the appearance of wrinkles and textural irregularities. Plus, it uses pro-vitamin B5 to enhance hydration at the outer layers, resulting in smoother, plumper skin.Clinical ResultsSmoothing serum that offers short and long-term hydration.Boosts skin hydration after 1 week (with sustained results after 4 weeks).Strengthens skin barrier after 4 weeks.Noticeably smoother and more supple skin after 4 weeks.Reduced appearance of fine lines and wrinkles after 4 weeks.**In a clinical study of 34 subjects applying product 2x/day for 4 weeks.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Use in AM Use in PM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12 months after opening.</t>
+  </si>
+  <si>
     <t xml:space="preserve">The Ordinary Niacinamide 10% + Zinc 1%</t>
   </si>
   <si>
     <t xml:space="preserve">Textural Irregularities, Dryness, Dullness, Visible Shine, Signs of Congestion</t>
   </si>
   <si>
-    <t xml:space="preserve">All Skin Types</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Water-based Serum</t>
-  </si>
-  <si>
     <t xml:space="preserve">Our Niacinamide 10% + Zinc 1% formula is a water-based serum that boosts skin brightness, improves skin smoothness and reinforces the skin barrier over time. It contains a high 10% concentration of Niacinamide (vitamin b3) and zinc PCA.Note: Niacinamide and Zinc PCA is not a treatment for acne. For persistent acne-related conditions, we recommend speaking to your health care provider regarding treatment options. This formulation can be used alongside acne treatments if desired for added visible skin benefits.Clinical ResultsHydrating lightweight serum that improves the look of skin radiance and luminosity.Hydrates skin by reinforcing the skin barrier in as little as 7 days.Achieve smoother skin after 8 weeks.**In a clinical study of 35 subjects applying product 2x/day for 8 weeks</t>
   </si>
   <si>
-    <t xml:space="preserve">Use in AM Use in PM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">12 months after opening.</t>
-  </si>
-  <si>
     <t xml:space="preserve">with Direct Vitamin C Indirect Vitamin C</t>
   </si>
   <si>
-    <t xml:space="preserve">The Ordinary Hyaluronic Acid 2% + B5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dryness</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hyaluronic Acid 2% + B5 is a water-based formula combining low-, medium- and high-molecular-weight hyaluronic acid molecules and a next-generation HA crosspolymer to support hydration to multiple layers of your skin. It also targets the appearance of wrinkles and textural irregularities. Plus, it uses pro-vitamin B5 to enhance hydration at the outer layers, resulting in smoother, plumper skin.Clinical ResultsSmoothing serum that offers short and long-term hydration.Boosts skin hydration after 1 week (with sustained results after 4 weeks).Strengthens skin barrier after 4 weeks.Noticeably smoother and more supple skin after 4 weeks.Reduced appearance of fine lines and wrinkles after 4 weeks.**In a clinical study of 34 subjects applying product 2x/day for 4 weeks.</t>
+    <t xml:space="preserve">The Ordinary Multi-Peptide + HA Serum</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Signs of Aging, Dryness, Crow's Feet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Multi-Peptide + HA Serum (formerly known as “Buffet”) is a universal formula that combines a comprehensive array of technologies to improve skin smoothness and target multiple signs of aging at once. By utilizing four well-studied peptide technologies, skin-friendly amino acids, and multiple hyaluronic acid complexes, it helps significantly improve the appearance of crow's feet, as well as improving the feel of skin elasticity and firmness.This formula contains SYN™-AKE, Matrixyl™ synthe'6™, Matrixyl™ 3000, ARGIRELOX™ peptide, Hyaluronic Acid, Amino Acids, and Bio-DerivativesAll trademarks belong to their respective owners. SYN™ is a trademark of DSM, Matrixyl™ synthe'6™ and Matrixyl™ 3000 are trademarks of Sederma Inc., and ARGIRELOX™ is a trademark of Lipotec S.A.U. Neither DECIEM nor The Ordinary is affiliated with the trademark owners.Clinical ResultsTargets common signs of aging such as the look of crow’s feet, firmness and elasticity.Reduces the appearance of crow’s feet wrinkles after 8 weeks*Improves the look of skin smoothness and texture*Promotes an improved appearance in skin’s elasticity and firmness**Independent efficacy study performed on 30 individuals over an 8 week period.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">with Direct Acids Direct Vitamin C Resveratrol and Ferulic Acid Salicylic Acid</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Ordinary Azelaic Acid Suspension 10%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Textural Irregularities, Dullness, Uneven Skin Tone, Look of Redness</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Suspension</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Azelaic Acid Suspension 10% is a cream-like formula that brightens skin tone and visibly improves skin texture due to a high concentration of azelaic acid—a natural and effective antioxidant found in grains. It has a lower irritation potential than other direct acids, which means it’s gentle enough for daily use as part of your skincare regimen.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">with Copper Peptides Direct Acids Direct Vitamin C EUK Niacinamide Powder Peptides Retinoids</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Ordinary Multi-Peptide Lash and Brow Serum</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hair</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Multi-Peptide Lash and Brow Serum is a light, non-greasy formula designed to support thicker, fuller, and healthier-looking lashes and brows. By utilizing 11 active ingredients, including four peptide complexes and a series of natural extracts, this twice-daily serum works to help nourish and protect your lashes and brows while enhancing the look of density and overall appearance in as little as four weeks.This formula contains SYMPEPTIDE XLASH® complex (with Myristoyl Pentapeptide-17), Anargy® complex (with Oligopeptide-2 and Glycoproteins), Widelash™ complex (with Biotinoyl Tripeptide-1 and Panthenol), REDENSYL™ complex (with Larix Europaea Wood Extract, Camellia Sinensis Leaf Extract, and Zinc Chloride), CAPIXYL™ complex (Acetyl Tetrapeptide-3 and Trifolium Pratense Flower Extract), and High-Solubility Caffeine.All trademarks belong to their respective owners. SYMPEPTIDE XLASH® is a registered trademark of SYMRISE AG, Anargy® is a registered trademark of LIPOTRUE, S.L., Widelash™ is a trademark of Sederma Inc., REDENSYL™ is a trademark of Givaudan, and CAPIXYL™ is a trademark of Lucas Meyer Cosmetics Canada Inc. Neither DECIEM nor The Ordinary is affiliated with the trademark owners. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">6 months after opening.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Ordinary Argireline Solution 10%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Signs of Aging, Crow's Feet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Argireline Solution 10% offers an advanced formula targeting dynamic forehead, “eleven eye”, and smile lines in an effective, “non-injective” way. By incorporating a high concentration of Argireline™ , this lightweight serum improves the appearance of facial areas prone to deep-set lines, resulting in smoother, more relaxed skin.ARGIRELINE™ is a trademark of Lipotec S.A.U. Neither DECIEM nor The Ordinary is affiliated with Lipotec S.A.U.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Ordinary Retinol 1% in Squalane</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Signs of Aging, Dryness, Textural Irregularities, Uneven Skin Tone</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Anhydrous Serum</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Retinol 1% in Squalane offers a water-free solution containing 1% retinol—an ingredient that improves the appearance of fine and dynamic lines that arise from a loss of collagen and elastin, while evening skin texture and tone. What’s more, this expert-level formula is supported with squalane, a moisturizing agent naturally found in your skin that enhances surface-level hydration and helps combat the dryness that can be associated with retinol use.The Ordinary Tip: Start with Retinol 0.2% in Squalane and slowly work your way up to Retinol 0.5% in Squalane and Retinol 1% in Squalane. That said, if you are prone to sensitivity, you may prefer to use newer retinoid technologies, such as those found in our Granactive Retinoid 2% Emulsion.Note: Once opened, this formula should be refrigerated and used within a three-month period.Caution: Retinoids can make the skin more sensitive to UV radiation. Sun protection is particularly important when using retinoids. This product must not be used in conjunction with other retinoids including retinol or retinoic acid. This product is not a treatment for acneNote: When pregnant or breastfeeding, it is recommended to avoid any skincare products containing retinoids such as formulations with Granactive Retinoid or Retinol.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Use in PM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3 months after opening.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">with Copper Peptides Direct Acids Direct Vitamin C Retinoids</t>
   </si>
   <si>
     <t xml:space="preserve">The Ordinary Matrixyl 10% + HA</t>
@@ -80,70 +149,133 @@
     <t xml:space="preserve">Matrixyl 10% + HA offers an advanced formula that targets fine lines and wrinkles by promoting firmer, plumper skin. With two generations of MatrixylTM and hyaluronic acid, this lightweight serum improves the appearance of facial areas prone to fine lines by supporting your skin’s overall collagen production.Matrixyl™ is a trademark of Sederma Inc. Neither DECIEM nor The Ordinary is affiliated with Sederma Inc. </t>
   </si>
   <si>
-    <t xml:space="preserve">with Direct Acids Direct Vitamin C Resveratrol and Ferulic Acid Salicylic Acid</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The Ordinary Multi-Peptide + HA Serum</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Signs of Aging, Dryness, Crow's Feet</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Multi-Peptide + HA Serum (formerly known as “Buffet”) is a universal formula that combines a comprehensive array of technologies to improve skin smoothness and target multiple signs of aging at once. By utilizing four well-studied peptide technologies, skin-friendly amino acids, and multiple hyaluronic acid complexes, it helps significantly improve the appearance of crow's feet, as well as improving the feel of skin elasticity and firmness.This formula contains SYN™-AKE, Matrixyl™ synthe'6™, Matrixyl™ 3000, ARGIRELOX™ peptide, Hyaluronic Acid, Amino Acids, and Bio-DerivativesAll trademarks belong to their respective owners. SYN™ is a trademark of DSM, Matrixyl™ synthe'6™ and Matrixyl™ 3000 are trademarks of Sederma Inc., and ARGIRELOX™ is a trademark of Lipotec S.A.U. Neither DECIEM nor The Ordinary is affiliated with the trademark owners.Clinical ResultsTargets common signs of aging such as the look of crow’s feet, firmness and elasticity.Reduces the appearance of crow’s feet wrinkles after 8 weeks*Improves the look of skin smoothness and texture*Promotes an improved appearance in skin’s elasticity and firmness**Independent efficacy study performed on 30 individuals over an 8 week period.</t>
+    <t xml:space="preserve">The Ordinary Alpha Arbutin 2% + HA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Uneven Skin Tone, Dryness</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Alpha Arbutin 2% + HA is a water-based serum specifically designed to target uneven skin tone and visibly improve pigmentation. It combines a high concentration of purified alpha arbutin, a well-known skin-brightening ingredient, with hyaluronic acid. Purified alpha-arbutin works to target dark spots and uneven skin tone. Meanwhile, hyaluronic acid helps to support product absorption into the skin.Note: Alpha Arbutin is extremely sensitive to degradation in the presence of water if the pH of the formulation is not ideal. The pH of this formula has been shown to be the most suitable pH to minimize degradation of Alpha Arbutin.We are aware of the potential colour changes of our Alpha Arbutin product. This is a natural occurrence, where certain ingredients in the product can change colour when exposed to sunlight or increased temperature. Testing has shown that the efficacy and safety profile of the active ingredient remains stable.</t>
   </si>
   <si>
     <t xml:space="preserve">The Ordinary “Buffet” + Copper Peptides 1%</t>
   </si>
   <si>
-    <t xml:space="preserve">Signs of Aging, Crow's Feet</t>
-  </si>
-  <si>
     <t xml:space="preserve">“Buffet” + Copper Peptides 1% is a universal formula which utilizes multiple skin support technologies that target multiple signs of aging at once. The formula incorporates five well-studied peptide technologies, skin-friendly amino acids, and multiple hyaluronic acids. For those looking for an all-in-one solution for skin care, “Buffet” + Copper Peptides 1% helps to improve the appearance of fine and dynamic lines and supports your skin’s overall elasticity, smoothness and firmness. And because this advanced serum contains direct copper peptides, it also targets signs of aging that are typically associated with oxidative stress, resulting in radiant, healthier-looking skin.This formula contains GHK-Cu, SYN™-AKE, Matrixyl™ synthe'6™, Matrixyl™ 3000, ARGIRELOX™ peptide, Hyaluronic Acid, Amino Acids, and Bio-DerivativesAll trademarks belong to their respective owners. SYN™ is a trademark of DSM, Matrixyl™ synthe'6™ and Matrixyl™ 3000 are trademarks of Sederma Inc., and ARGIRELOX™ is a trademark of Lipotec S.A.U. Neither DECIEM nor The Ordinary is affiliated with the trademark owners.</t>
   </si>
   <si>
-    <t xml:space="preserve">6 months after opening.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">with Direct Acids Direct Vitamin C EUK Retinoids Strong Antioxidants Resveratrol and Ferulic Acid Salicylic Acid</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The Ordinary Argireline Solution 10%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Argireline Solution 10% offers an advanced formula targeting dynamic forehead, “eleven eye”, and smile lines in an effective, “non-injective” way. By incorporating a high concentration of Argireline™ , this lightweight serum improves the appearance of facial areas prone to deep-set lines, resulting in smoother, more relaxed skin.ARGIRELINE™ is a trademark of Lipotec S.A.U. Neither DECIEM nor The Ordinary is affiliated with Lipotec S.A.U.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The Ordinary Multi-Peptide Lash and Brow Serum</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hair</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The Multi-Peptide Lash and Brow Serum is a light, non-greasy formula designed to support thicker, fuller, and healthier-looking lashes and brows. By utilizing 11 active ingredients, including four peptide complexes and a series of natural extracts, this twice-daily serum works to help nourish and protect your lashes and brows while enhancing the look of density and overall appearance in as little as four weeks.This formula contains SYMPEPTIDE XLASH® complex (with Myristoyl Pentapeptide-17), Anargy® complex (with Oligopeptide-2 and Glycoproteins), Widelash™ complex (with Biotinoyl Tripeptide-1 and Panthenol), REDENSYL™ complex (with Larix Europaea Wood Extract, Camellia Sinensis Leaf Extract, and Zinc Chloride), CAPIXYL™ complex (Acetyl Tetrapeptide-3 and Trifolium Pratense Flower Extract), and High-Solubility Caffeine.All trademarks belong to their respective owners. SYMPEPTIDE XLASH® is a registered trademark of SYMRISE AG, Anargy® is a registered trademark of LIPOTRUE, S.L., Widelash™ is a trademark of Sederma Inc., REDENSYL™ is a trademark of Givaudan, and CAPIXYL™ is a trademark of Lucas Meyer Cosmetics Canada Inc. Neither DECIEM nor The Ordinary is affiliated with the trademark owners. </t>
+    <t xml:space="preserve">with Direct Acids Direct Vitamin C Resveratrol and Ferulic Acid Salicylic Acid EUK Retinoids Strong Antioxidants</t>
   </si>
   <si>
     <t xml:space="preserve">The Ordinary Granactive Retinoid 5% in Squalane</t>
   </si>
   <si>
-    <t xml:space="preserve">Textural Irregularities, Signs of Aging, Uneven Skin Tone</t>
+    <t xml:space="preserve">Signs of Aging, Textural Irregularities, Uneven Skin Tone</t>
   </si>
   <si>
     <t xml:space="preserve">Dry Skin</t>
   </si>
   <si>
-    <t xml:space="preserve">Anhydrous Serum</t>
-  </si>
-  <si>
     <t xml:space="preserve">Granactive Retinoid 5% in Squalane is a light, oil-like serum that targets visible signs of aging through a highly-advanced retinoid active, one of the best all-around ingredients for skin. This next-generation retinoid improves the appearance of fine and dynamic lines that arise from a loss of collagen and elastin while evening skin texture and tone. It’s further supported with squalane, a moisturizing agent naturally found in the skin. That means it not only delivers comparable visible results to retinol, it’s less likely to cause irritation.Granactive Retinoid™ is a trademark of Grant Industries. Neither DECIEM nor The Ordinary is affiliated with Grant Industries.Note: Once opened, this formula should be refrigerated and used within a three-month period.Caution: Retinoids can make the skin more sensitive to UV radiation. Sun protection is particularly important when using retinoids. This product must not be used in conjunction with other retinoids including retinol or retinoic acid. This product is not a treatment for acne.Note: When pregnant or breastfeeding, it is recommended to avoid any skincare products containing retinoids such as formulations with Granactive Retinoid or Retinol.</t>
   </si>
   <si>
-    <t xml:space="preserve">Use in PM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3 months after opening.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">with Copper Peptides Direct Acids Direct Vitamin C Retinoids</t>
+    <t xml:space="preserve">Aloe 2% + NAG 2% Solution</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Textural Irregularities, Uneven Skin Tone, Look of Redness</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aloe 2% + NAG 2% Solution is a lightweight soothing serum formulated for blemish-prone skin. It reduces the appearance of post-acne marks through the inclusion of ingredients that target the look and feel of both uneven skin tone and texture, while also helping to reduce the appearance of pores, and strengthening skin barrier.This formulation incorporates aloe barbadensis leaf juice powder for hydration. It also contains N-acetyl glucosamine (NAG), a biotechnology-derived ingredient that has been shown to effectively target the appearance of uneven skin tone. It is further supported by peptide technology palmitoyl pentapeptide-4 which targets the feel of textural irregularities, while offering effective barrier support.Testing ShowsReduces the appearance of post-acne marksReduces the look of skin redness caused by irritationReduces the appearance of poresImproves the appearance of uneven skin tone and the feel of uneven skin textureStrengthens and maintains skin barrier functionBoosts skin hydration*Consumer testing on 31 subjects after using product 2x/day for 8 weeks.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Ordinary Retinol 0.5% in Squalane</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Retinol 0.5% in Squalane offers a water-free solution containing 0.5% retinol—an ingredient that improves the appearance of fine and dynamic lines that arise from a loss of collagen and elastin, while evening skin texture and tone. What’s more, this intermediate formula is supported with squalane, a moisturizing agent naturally found in your skin that enhances surface-level hydration and helps combat the dryness that can be associated with retinol use.  The Ordinary Tip: Start with Retinol 0.2% in Squalane and slowly work your way up to Retinol 0.5% in Squalane and Retinol 1% in Squalane. That said, if you are prone to sensitivity, you may prefer to use newer retinoid technologies, such as those found in our Granactive Retinoid 2% Emulsion.  Note: Once opened, this formula should be refrigerated and used within a three-month period.  Caution: Retinoids can make the skin more sensitive to UV radiation. Sun protection is particularly important when using retinoids. This product must not be used in conjunction with other retinoids including retinol or retinoic acid. This product is not a treatment for acne.   Note: When pregnant or breastfeeding, it is recommended to avoid any skincare products containing retinoids such as formulations with Granactive Retinoid or Retinol.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Ordinary Vitamin C Suspension 30% in Silicone</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dullness, Signs of Aging, Antioxidant Support, Uneven Skin Tone</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vitamin C Suspension 30% in Silicone is a smooth cream-like formula that uses direct Vitamin C to help visibly reduce signs of aging by brightening and balancing uneven skin tone. This water-free formula provides 30% direct L-Ascorbic Acid which remains completely stable due to the absence of water. What’s more, this water-free formula contains extra-light silicones, which lessen the tingling sensation that can be associated with topical vitamin C treatments.  Note: The vitamin C powder in this formula may contribute to the texture of the product which is suspended in a silicone base, providing a smooth and soft skin feel. If desired, this formula can be diluted in a cream base per application to allow the skin to build tolerance over time.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">with Copper Peptides Direct Acids Direct Vitamin C EUK Niacinamide Peptides Retinoids</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Ordinary Granactive Retinoid 2% in Squalane</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Granactive Retinoid 2% in Squalane is a light, oil-like serum that targets visible signs of aging through a highly-advanced retinoid active, one of the best all-around ingredients for skin. This next-generation retinoid improves the appearance of fine and dynamic lines that arise from a loss of collagen and elastin while evening skin texture and tone. It’s further supported with squalane, a moisturizing agent naturally found in the skin. That means it not only delivers comparable visible results to retinol, it’s less likely to cause irritation.Granactive Retinoid™ is a trademark of Grant Industries. Neither DECIEM nor The Ordinary is affiliated with Grant Industries.Note: Once opened, this formula should be refrigerated and used within a three-month period.Caution: Retinoids can make the skin more sensitive to UV radiation. Sun protection is particularly important when using retinoids. This product must not be used in conjunction with other retinoids including retinol or retinoic acid. This product is not a treatment for acne.Note: When pregnant or breastfeeding, it is recommended to avoid any skincare products containing retinoids such as formulations with Granactive Retinoid or Retinol.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Ordinary Amino Acids + B5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Amino Acids + B5 is an ultra-thin serum that works with your skin to support its natural hydration barrier. By including a concentrated 17% (by weight) solution of amino acids and amino acid derivatives that mimic your skin’s natural moisturizing factors, this water-based formula keeps the outer layer of your skin protected and well-hydrated without feeling greasy. Plus, it uses 5% (by weight) pro-vitamin B5 to provide surface and below-surface hydration, giving way to softer, smoother skin.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Ordinary Ascorbyl Tetraisopalmitate Solution 20% in Vitamin F</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ascorbyl Tetraisopalmitate Solution 20% in Vitamin F is a lightweight oil that helps reduce signs of aging by brightening and balancing uneven skin tone. Unlike direct forms of vitamin C, this hydrating formula contains an oil-soluble vitamin C derivative that converts into vitamin C once applied, giving it less irritation potential. Plus, it has vitamin F—Omega 3 and Omega 6 fatty acids—to help support your skin’s natural hydration barrier. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">6 months after opening</t>
+  </si>
+  <si>
+    <t xml:space="preserve">with Niacinamide</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Ordinary Resveratol 3% + Ferulic Acid 3%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Antioxidant Support, Dullness</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Resveratrol 3% + Ferulic Acid 3% serum is a light, oil-like serum for daily skin protection from the impact of oxidative stress. Using two well-known antioxidants, this formula helps protect your skin from the visual effects of damage caused by environmental stressors, visible signs of aging, and helps it to look brighter and smoother.  Since water can impair the stability of antioxidants, Resveratrol 3% + Ferulic Acid 3% is a water-free formula. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">with Copper Peptides EUK Peptides Re: Pigment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Ordinary Ascorbyl Glucoside Solution 12%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ascorbyl Glucoside Solution 12% offers a lightweight, water-based formula that helps reduce signs of aging by brightening and balancing uneven skin tone. Unlike direct forms of vitamin C, this easy-to-use serum contains a water-soluble vitamin C derivative that converts into vitamin C once applied, giving it less irritation potential. And because it has advanced antioxidant properties, it also protects skin from the visual effects of damage caused by environmental stressors, helping to maintain a more radiant complexion.   Note: In its pure form, vitamin C is unstable in water. Ascorbyl Glucoside is a water-soluble derivative of vitamin C. It is much more stable in water but it is less potent than direct L-Ascorbic Acid. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Ordinary Granactive Retinoid 2% Emulsion</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Emulsion</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Granactive Retinoid 2% Emulsion is a creamy serum that targets visible signs of aging through a highly-advanced retinoid active, one of the best all-around ingredients for skin. This next-generation retinoid improves the appearance of fine and dynamic lines that arise from a loss of collagen and elastin, while evening skin texture and tone. What’s more, this advanced ingredient is not only proven to deliver comparable visible results to retinol; it’s less likely to cause irritation.Granactive Retinoid™ is a trademark of Grant Industries. Neither DECIEM nor The Ordinary is affiliated with Grant Industries.Note: Once opened, this formula should be refrigerated and used within a three-month period.Caution: Retinoids can make the skin more sensitive to UV radiation. Sun protection is particularly important when using retinoids. This product must not be used in conjunction with other retinoids including retinol or retinoic acid. This product is not a treatment for acne.Note: When pregnant or breastfeeding, it is recommended to avoid any skincare products containing retinoids such as formulations with Granactive Retinoid or Retinol.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Ordinary Ethylated Ascorbic Acid 15% Solution</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ethylated Ascorbic Acid 15% Solution is an advanced, direct-acting oil-like serum that helps visibly reduce signs of aging by brightening and balancing uneven skin tone. Among our other vitamin C offerings, what sets this formula apart is its ethylation which gives a small molecular size, allowing for faster visible results with less irritation potential. Ethylation is a process which helps promote the stability of Vitamin C while still retaining the direct-acting benefits when compared to other Vitamin C Derivatives. And because it has advanced antioxidant properties, this water-free formula protects your skin from the visual effects of damage caused by environmental stressors, helping to maintain a more radiant complexion.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Ordinary Vitamin C Suspension 23% + HA Spheres 2%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vitamin C Suspension 23% in HA Spheres uses direct vitamin C and hyaluronic acid to help visibly reduce signs of aging by brightening and balancing uneven skin tone. This water-free formula provides 23% pure L-Ascorbic Acid which remains completely stable due to the absence of water. What’s more, this water-free formula is supported with spheres of hyaluronic acid for added hydration.Note: The slightly granular texture of this product is due to the vitamin C powder being suspended in an oil-like base and therefore each application requires a few seconds to feel absorbed by the skin. If desired, this formula can be diluted in a cream base per application to allow the skin to build tolerance over time.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Ordinary 100% Plant-Derived Squalane</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dryness, Hair</t>
+  </si>
+  <si>
+    <t xml:space="preserve">100% Plant-Derived Squalane hydrates your skin while supporting its natural moisture barrier. Squalane is an exceptional hydrator found naturally in the skin, and this formula uses 100% plant-derived squalane derived from sugar cane for a non-comedogenic solution that enhances surface-level hydration.Our 100% Plant-Derived Squalane formula can also be used in hair to increase heat protection, add shine, and reduce breakage.</t>
   </si>
   <si>
     <t xml:space="preserve">The Ordinary Marine Hyaluronics</t>
@@ -152,196 +284,64 @@
     <t xml:space="preserve">Marine Hyaluronics offers an exceptionally lightweight serum, acting as a hyaluronic acid-alternative, which directs water where you need it most. By combining exopolysaccharides from skin-friendly marine bacteria, Hawaiian red algae, glycoproteins from Antarctic marine sources, micro-filtered blue-green algae, and several amino acids, this water-based formula targets hydration below the skin surface, resulting in a softer, plumper complexion. </t>
   </si>
   <si>
-    <t xml:space="preserve">The Ordinary Azelaic Acid Suspension 10%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Textural Irregularities, Dullness, Uneven Skin Tone, Look of Redness</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Suspension</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Azelaic Acid Suspension 10% is a cream-like formula that brightens skin tone and visibly improves skin texture due to a high concentration of azelaic acid—a natural and effective antioxidant found in grains. It has a lower irritation potential than other direct acids, which means it’s gentle enough for daily use as part of your skincare regimen.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">with Copper Peptides Direct Acids Direct Vitamin C EUK Niacinamide Powder Peptides Retinoids</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The Ordinary Granactive Retinoid 2% Emulsion</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Emulsion</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Granactive Retinoid 2% Emulsion is a creamy serum that targets visible signs of aging through a highly-advanced retinoid active, one of the best all-around ingredients for skin. This next-generation retinoid improves the appearance of fine and dynamic lines that arise from a loss of collagen and elastin, while evening skin texture and tone. What’s more, this advanced ingredient is not only proven to deliver comparable visible results to retinol; it’s less likely to cause irritation.Granactive Retinoid™ is a trademark of Grant Industries. Neither DECIEM nor The Ordinary is affiliated with Grant Industries.Note: Once opened, this formula should be refrigerated and used within a three-month period.Caution: Retinoids can make the skin more sensitive to UV radiation. Sun protection is particularly important when using retinoids. This product must not be used in conjunction with other retinoids including retinol or retinoic acid. This product is not a treatment for acne.Note: When pregnant or breastfeeding, it is recommended to avoid any skincare products containing retinoids such as formulations with Granactive Retinoid or Retinol.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The Ordinary Amino Acids + B5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Amino Acids + B5 is an ultra-thin serum that works with your skin to support its natural hydration barrier. By including a concentrated 17% (by weight) solution of amino acids and amino acid derivatives that mimic your skin’s natural moisturizing factors, this water-based formula keeps the outer layer of your skin protected and well-hydrated without feeling greasy. Plus, it uses 5% (by weight) pro-vitamin B5 to provide surface and below-surface hydration, giving way to softer, smoother skin.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The Ordinary Retinol 0.5% in Squalane</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Textural Irregularities, Dryness, Signs of Aging, Uneven Skin Tone</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Retinol 0.5% in Squalane offers a water-free solution containing 0.5% retinol—an ingredient that improves the appearance of fine and dynamic lines that arise from a loss of collagen and elastin, while evening skin texture and tone. What’s more, this intermediate formula is supported with squalane, a moisturizing agent naturally found in your skin that enhances surface-level hydration and helps combat the dryness that can be associated with retinol use.  The Ordinary Tip: Start with Retinol 0.2% in Squalane and slowly work your way up to Retinol 0.5% in Squalane and Retinol 1% in Squalane. That said, if you are prone to sensitivity, you may prefer to use newer retinoid technologies, such as those found in our Granactive Retinoid 2% Emulsion.  Note: Once opened, this formula should be refrigerated and used within a three-month period.  Caution: Retinoids can make the skin more sensitive to UV radiation. Sun protection is particularly important when using retinoids. This product must not be used in conjunction with other retinoids including retinol or retinoic acid. This product is not a treatment for acne.   Note: When pregnant or breastfeeding, it is recommended to avoid any skincare products containing retinoids such as formulations with Granactive Retinoid or Retinol.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The Ordinary Retinol 1% in Squalane</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Retinol 1% in Squalane offers a water-free solution containing 1% retinol—an ingredient that improves the appearance of fine and dynamic lines that arise from a loss of collagen and elastin, while evening skin texture and tone. What’s more, this expert-level formula is supported with squalane, a moisturizing agent naturally found in your skin that enhances surface-level hydration and helps combat the dryness that can be associated with retinol use.The Ordinary Tip: Start with Retinol 0.2% in Squalane and slowly work your way up to Retinol 0.5% in Squalane and Retinol 1% in Squalane. That said, if you are prone to sensitivity, you may prefer to use newer retinoid technologies, such as those found in our Granactive Retinoid 2% Emulsion.Note: Once opened, this formula should be refrigerated and used within a three-month period.Caution: Retinoids can make the skin more sensitive to UV radiation. Sun protection is particularly important when using retinoids. This product must not be used in conjunction with other retinoids including retinol or retinoic acid. This product is not a treatment for acneNote: When pregnant or breastfeeding, it is recommended to avoid any skincare products containing retinoids such as formulations with Granactive Retinoid or Retinol.</t>
-  </si>
-  <si>
     <t xml:space="preserve">The Ordinary Retinol 0.2% in Squalane</t>
   </si>
   <si>
     <t xml:space="preserve">Retinol 0.2% in Squalane offers a water-free solution containing 0.2% retinol—an ingredient that improves the appearance of fine and dynamic lines that arise from a loss of collagen and elastin, while evening skin texture and tone. What’s more, this entry-level formula is supported with squalane, a moisturizing agent naturally found in your skin that enhances surface-level hydration and helps combat the dryness that can be associated with retinol use.  The Ordinary Tip: Start with Retinol 0.2% in Squalane and slowly work your way up to Retinol 0.5% in Squalane and Retinol 1% in Squalane. That said, if you are prone to sensitivity, you may prefer to use newer retinoid technologies, such as those found in our Granactive Retinoid 2% Emulsion.  Note: Once opened, this formula should be refrigerated and used within a three-month period.  Caution: Retinoids can make the skin more sensitive to UV radiation. Sun protection is particularly important when using retinoids. This product must not be used in conjunction with other retinoids including retinol or retinoic acid. This product is not a treatment for acne.   Note: When pregnant or breastfeeding, it is recommended to avoid any skincare products containing retinoids such as formulations with Granactive Retinoid or Retinol.</t>
   </si>
   <si>
+    <t xml:space="preserve">The Ordinary Pycnogenol 5%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pycnogenol 5% offers an oil-like formula that helps support your skin against the impact of oxidative stress. Incorporating an exclusive French maritime pine bark extract, this vibrant serum aims to brighten skin and is a deep red color due to the high antioxidant (procyanidins) content. It works to protect your skin from the visible effects of damage caused by environmental aggressors.Note: Pycnogenol® is known to support the antioxidant activity of ascorbic acid, making this formula an ideal accompaniment to regimens that already incorporate vitamin C.Pycnogenol® is a registered trademark of Horphag Research Ltd. Neither DECIEM nor The Ordinary is affiliated with Horphag Research Ltd. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">with Copper Peptides</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Ordinary EUK 134 0.1%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EUK 134™ 0.1%, is an oil-like serum designed to continuously support your skin with antioxidants and leave your skin looking brighter. By using a self-regenerating molecule that mimics the effects of two powerful antioxidants found naturally in your skin, this high-strength serum actively protects your skin from the visible effects of damage caused by environmental stressors.   The low price of this formula does not reflect EUK-134™'s extremely high potency. EUK-134™ is by far one of the strongest antioxidants available. While EUK-134™ itself is very costly, the suggested concentration in any formula is below 0.05% and most formulas do not use this maximum suggestion. Our formula uses EUK-134™ at an extremely high 0.1% concentration and we do not believe any product on the market today uses a higher concentration than this amount.  EUK-134™ is a trademark of Lucas Meyer Cosmetics Canada Inc. Neither DECIEM nor The Ordinary is affiliated with Lucas Meyer Cosmetics Canada Inc.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">with Copper Peptides Direct Acids Direct Vitamin C Resveratrol and Ferulic Acid</t>
+  </si>
+  <si>
     <t xml:space="preserve">The Ordinary 100% Plant-Derived Hemi-Squalane</t>
   </si>
   <si>
-    <t xml:space="preserve">Dryness, Hair</t>
-  </si>
-  <si>
     <t xml:space="preserve">A fast-absorbing hydrator, 100% Plant-Derived Hemi-Squalane supports your skin’s natural moisture barrier with an exceptionally light texture that allows for a dry skin finish.This product offers a more lightweight texture and feel than our 100% Plant-Derived Squalane.Our 100% Plant-Derived Hemi-Squalane can also be used in hair to decrease frizz.</t>
   </si>
   <si>
-    <t xml:space="preserve">The Ordinary Vitamin C Suspension 30% in Silicone</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dullness, Signs of Aging, Antioxidant Support, Uneven Skin Tone</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vitamin C Suspension 30% in Silicone is a smooth cream-like formula that uses direct Vitamin C to help visibly reduce signs of aging by brightening and balancing uneven skin tone. This water-free formula provides 30% direct L-Ascorbic Acid which remains completely stable due to the absence of water. What’s more, this water-free formula contains extra-light silicones, which lessen the tingling sensation that can be associated with topical vitamin C treatments.  Note: The vitamin C powder in this formula may contribute to the texture of the product which is suspended in a silicone base, providing a smooth and soft skin feel. If desired, this formula can be diluted in a cream base per application to allow the skin to build tolerance over time.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">with Copper Peptides Direct Acids Direct Vitamin C EUK Niacinamide Peptides Retinoids</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The Ordinary Ascorbyl Glucoside Solution 12%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ascorbyl Glucoside Solution 12% offers a lightweight, water-based formula that helps reduce signs of aging by brightening and balancing uneven skin tone. Unlike direct forms of vitamin C, this easy-to-use serum contains a water-soluble vitamin C derivative that converts into vitamin C once applied, giving it less irritation potential. And because it has advanced antioxidant properties, it also protects skin from the visual effects of damage caused by environmental stressors, helping to maintain a more radiant complexion.   Note: In its pure form, vitamin C is unstable in water. Ascorbyl Glucoside is a water-soluble derivative of vitamin C. It is much more stable in water but it is less potent than direct L-Ascorbic Acid. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">with Niacinamide</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The Ordinary Resveratol 3% + Ferulic Acid 3%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Antioxidant Support, Dullness</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Resveratrol 3% + Ferulic Acid 3% serum is a light, oil-like serum for daily skin protection from the impact of oxidative stress. Using two well-known antioxidants, this formula helps protect your skin from the visual effects of damage caused by environmental stressors, visible signs of aging, and helps it to look brighter and smoother.  Since water can impair the stability of antioxidants, Resveratrol 3% + Ferulic Acid 3% is a water-free formula. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">with Copper Peptides EUK Peptides Re: Pigment</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The Ordinary Granactive Retinoid 2% in Squalane</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Granactive Retinoid 2% in Squalane is a light, oil-like serum that targets visible signs of aging through a highly-advanced retinoid active, one of the best all-around ingredients for skin. This next-generation retinoid improves the appearance of fine and dynamic lines that arise from a loss of collagen and elastin while evening skin texture and tone. It’s further supported with squalane, a moisturizing agent naturally found in the skin. That means it not only delivers comparable visible results to retinol, it’s less likely to cause irritation.Granactive Retinoid™ is a trademark of Grant Industries. Neither DECIEM nor The Ordinary is affiliated with Grant Industries.Note: Once opened, this formula should be refrigerated and used within a three-month period.Caution: Retinoids can make the skin more sensitive to UV radiation. Sun protection is particularly important when using retinoids. This product must not be used in conjunction with other retinoids including retinol or retinoic acid. This product is not a treatment for acne.Note: When pregnant or breastfeeding, it is recommended to avoid any skincare products containing retinoids such as formulations with Granactive Retinoid or Retinol.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The Ordinary Pycnogenol 5%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pycnogenol 5% offers an oil-like formula that helps support your skin against the impact of oxidative stress. Incorporating an exclusive French maritime pine bark extract, this vibrant serum aims to brighten skin and is a deep red color due to the high antioxidant (procyanidins) content. It works to protect your skin from the visible effects of damage caused by environmental aggressors.Note: Pycnogenol® is known to support the antioxidant activity of ascorbic acid, making this formula an ideal accompaniment to regimens that already incorporate vitamin C.Pycnogenol® is a registered trademark of Horphag Research Ltd. Neither DECIEM nor The Ordinary is affiliated with Horphag Research Ltd. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">with Copper Peptides</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The Ordinary Vitamin C Suspension 23% + HA Spheres 2%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vitamin C Suspension 23% in HA Spheres uses direct vitamin C and hyaluronic acid to help visibly reduce signs of aging by brightening and balancing uneven skin tone. This water-free formula provides 23% pure L-Ascorbic Acid which remains completely stable due to the absence of water. What’s more, this water-free formula is supported with spheres of hyaluronic acid for added hydration.Note: The slightly granular texture of this product is due to the vitamin C powder being suspended in an oil-like base and therefore each application requires a few seconds to feel absorbed by the skin. If desired, this formula can be diluted in a cream base per application to allow the skin to build tolerance over time.</t>
+    <t xml:space="preserve">The Ordinary 100% Niacinamide Powder</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Textural Irregularities, Dullness, Visible Shine</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Powder</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This ultra-fine 100% Niacinamide Powder promotes a brighter, more radiant complexion by smoothing textural irregularities, mattifying the skin and minimizing oils. As a powder that is comprised of 100% niacinamide (commonly known as vitamin B3), it’s designed to be mixed with other water-based serums, creams or moisturizers in your skincare routine—allowing you to create a custom niacinamide treatment.  Mixing Guide: In its truest form, Niacinamide is readily water-soluble and dissolves in water-based products, such as serums and creams, with ease. The Ordinary’s 100% Niacinamide Powder can be mixed into any non-conflicting, water-based treatment, provided that the pH of the base is between 5.0 and 7.0. When it comes to the choice of a water-based base to mix with this formula, there are several options available within The Ordinary brand. These include the following:Hyaluronic Acid 2% + B5Natural Moisturizing Factors + HA“Buffet” + Copper Peptides 1%Matrixyl 10% + HAArgireline Solution 10%To give an example of how to mix the product, if 1/4 scoop of the powder consists approximately of 0.05g Niacinamide, when mixed with 4 drops of the selected base, the resulting mixture is estimated to yield a 10-15% concentration of Niacinamide.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Refer to expiration date on product.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">with Direct Vitamin C Indirect Vitamin C Direct Acids</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Ordinary 100% L-Ascorbic Acid Powder</t>
+  </si>
+  <si>
+    <t xml:space="preserve">100% L-Ascorbic Acid Powder is a powdered form of direct vitamin C that visibly reduces signs of aging by brightening and balancing uneven skin tone and protecting your skin from the effects of damage caused by environmental stressors. Because it’s made of 100% vitamin C, it’s designed to be mixed with other serums, creams, or moisturizers in your skincare routine—allowing you to create a custom vitamin C treatment.  Depending on your mixture, your combination may offer a high concentration of direct vitamin c and as a result, a very strong tingling but non-irritating sensation is expected during the first 1-2 weeks of use until the skin's tolerance to such high exposure is elevated.</t>
   </si>
   <si>
     <t xml:space="preserve">The Ordinary Ascorbic Acid 8% + Alpha Arbutin 2%</t>
   </si>
   <si>
     <t xml:space="preserve">Ascorbic Acid 8% + Alpha Arbutin 2% is made with two of the most well-known brightening agents in skincare. Its water-free formula combines direct vitamin C and a high concentration of alpha arbutin to visibly improve pigmentation and balance uneven skin tone. With advanced antioxidant properties, it protects the skin from the visual effects of damage caused by environmental stressors, helping to maintain a more radiant complexion.Note: Vitamin C and Alpha Arbutin are less stable in formulations that contain water and use of them combined in formulations containing water is highly discouraged. This formulation is a water-free, stable solution, and may feel slightly "oily" for a few seconds after application, despite the fact that it is completely free of oil.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The Ordinary Alpha Arbutin 2% + HA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Uneven Skin Tone, Dryness</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Alpha Arbutin 2% + HA is a water-based serum specifically designed to target uneven skin tone and visibly improve pigmentation. It combines a high concentration of purified alpha arbutin, a well-known skin-brightening ingredient, with hyaluronic acid. Purified alpha-arbutin works to target dark spots and uneven skin tone. Meanwhile, hyaluronic acid helps to support product absorption into the skin.Note: Alpha Arbutin is extremely sensitive to degradation in the presence of water if the pH of the formulation is not ideal. The pH of this formula has been shown to be the most suitable pH to minimize degradation of Alpha Arbutin.We are aware of the potential colour changes of our Alpha Arbutin product. This is a natural occurrence, where certain ingredients in the product can change colour when exposed to sunlight or increased temperature. Testing has shown that the efficacy and safety profile of the active ingredient remains stable.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The Ordinary 100% Plant-Derived Squalane</t>
-  </si>
-  <si>
-    <t xml:space="preserve">100% Plant-Derived Squalane hydrates your skin while supporting its natural moisture barrier. Squalane is an exceptional hydrator found naturally in the skin, and this formula uses 100% plant-derived squalane derived from sugar cane for a non-comedogenic solution that enhances surface-level hydration.Our 100% Plant-Derived Squalane formula can also be used in hair to increase heat protection, add shine, and reduce breakage.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Aloe 2% + NAG 2% Solution</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Textural Irregularities, Uneven Skin Tone, Look of Redness</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Aloe 2% + NAG 2% Solution is a lightweight soothing serum formulated for blemish-prone skin. It reduces the appearance of post-acne marks through the inclusion of ingredients that target the look and feel of both uneven skin tone and texture, while also helping to reduce the appearance of pores, and strengthening skin barrier.This formulation incorporates aloe barbadensis leaf juice powder for hydration. It also contains N-acetyl glucosamine (NAG), a biotechnology-derived ingredient that has been shown to effectively target the appearance of uneven skin tone. It is further supported by peptide technology palmitoyl pentapeptide-4 which targets the feel of textural irregularities, while offering effective barrier support.Testing ShowsReduces the appearance of post-acne marksReduces the look of skin redness caused by irritationReduces the appearance of poresImproves the appearance of uneven skin tone and the feel of uneven skin textureStrengthens and maintains skin barrier functionBoosts skin hydration*Consumer testing on 31 subjects after using product 2x/day for 8 weeks.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The Ordinary EUK 134 0.1%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EUK 134™ 0.1%, is an oil-like serum designed to continuously support your skin with antioxidants and leave your skin looking brighter. By using a self-regenerating molecule that mimics the effects of two powerful antioxidants found naturally in your skin, this high-strength serum actively protects your skin from the visible effects of damage caused by environmental stressors.   The low price of this formula does not reflect EUK-134™'s extremely high potency. EUK-134™ is by far one of the strongest antioxidants available. While EUK-134™ itself is very costly, the suggested concentration in any formula is below 0.05% and most formulas do not use this maximum suggestion. Our formula uses EUK-134™ at an extremely high 0.1% concentration and we do not believe any product on the market today uses a higher concentration than this amount.  EUK-134™ is a trademark of Lucas Meyer Cosmetics Canada Inc. Neither DECIEM nor The Ordinary is affiliated with Lucas Meyer Cosmetics Canada Inc.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">with Copper Peptides Direct Acids Direct Vitamin C Resveratrol and Ferulic Acid</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The Ordinary 100% L-Ascorbic Acid Powder</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Powder</t>
-  </si>
-  <si>
-    <t xml:space="preserve">100% L-Ascorbic Acid Powder is a powdered form of direct vitamin C that visibly reduces signs of aging by brightening and balancing uneven skin tone and protecting your skin from the effects of damage caused by environmental stressors. Because it’s made of 100% vitamin C, it’s designed to be mixed with other serums, creams, or moisturizers in your skincare routine—allowing you to create a custom vitamin C treatment.  Depending on your mixture, your combination may offer a high concentration of direct vitamin c and as a result, a very strong tingling but non-irritating sensation is expected during the first 1-2 weeks of use until the skin's tolerance to such high exposure is elevated.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The Ordinary Ethylated Ascorbic Acid 15% Solution</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ethylated Ascorbic Acid 15% Solution is an advanced, direct-acting oil-like serum that helps visibly reduce signs of aging by brightening and balancing uneven skin tone. Among our other vitamin C offerings, what sets this formula apart is its ethylation which gives a small molecular size, allowing for faster visible results with less irritation potential. Ethylation is a process which helps promote the stability of Vitamin C while still retaining the direct-acting benefits when compared to other Vitamin C Derivatives. And because it has advanced antioxidant properties, this water-free formula protects your skin from the visual effects of damage caused by environmental stressors, helping to maintain a more radiant complexion.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The Ordinary 100% Niacinamide Powder</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Textural Irregularities, Dullness, Visible Shine</t>
-  </si>
-  <si>
-    <t xml:space="preserve">This ultra-fine 100% Niacinamide Powder promotes a brighter, more radiant complexion by smoothing textural irregularities, mattifying the skin and minimizing oils. As a powder that is comprised of 100% niacinamide (commonly known as vitamin B3), it’s designed to be mixed with other water-based serums, creams or moisturizers in your skincare routine—allowing you to create a custom niacinamide treatment.  Mixing Guide: In its truest form, Niacinamide is readily water-soluble and dissolves in water-based products, such as serums and creams, with ease. The Ordinary’s 100% Niacinamide Powder can be mixed into any non-conflicting, water-based treatment, provided that the pH of the base is between 5.0 and 7.0. When it comes to the choice of a water-based base to mix with this formula, there are several options available within The Ordinary brand. These include the following:Hyaluronic Acid 2% + B5Natural Moisturizing Factors + HA“Buffet” + Copper Peptides 1%Matrixyl 10% + HAArgireline Solution 10%To give an example of how to mix the product, if 1/4 scoop of the powder consists approximately of 0.05g Niacinamide, when mixed with 4 drops of the selected base, the resulting mixture is estimated to yield a 10-15% concentration of Niacinamide.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Refer to expiration date on product.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">with Direct Vitamin C Indirect Vitamin C Direct Acids</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The Ordinary Ascorbyl Tetraisopalmitate Solution 20% in Vitamin F</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ascorbyl Tetraisopalmitate Solution 20% in Vitamin F is a lightweight oil that helps reduce signs of aging by brightening and balancing uneven skin tone. Unlike direct forms of vitamin C, this hydrating formula contains an oil-soluble vitamin C derivative that converts into vitamin C once applied, giving it less irritation potential. Plus, it has vitamin F—Omega 3 and Omega 6 fatty acids—to help support your skin’s natural hydration barrier. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">6 months after opening</t>
   </si>
 </sst>
 </file>
@@ -389,8 +389,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A1:H32" totalsRowCount="0" totalsRowShown="0">
-  <autoFilter ref="A1:H32"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A1:H36" totalsRowCount="0" totalsRowShown="0">
+  <autoFilter ref="A1:H36"/>
   <tableColumns count="8">
     <tableColumn id="1" name="product_name"/>
     <tableColumn id="2" name="target"/>
@@ -738,16 +738,14 @@
       <c r="G2" t="s">
         <v>14</v>
       </c>
-      <c r="H2" t="s">
-        <v>15</v>
-      </c>
+      <c r="H2"/>
     </row>
     <row r="3">
       <c r="A3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" t="s">
         <v>16</v>
-      </c>
-      <c r="B3" t="s">
-        <v>17</v>
       </c>
       <c r="C3" t="s">
         <v>10</v>
@@ -756,7 +754,7 @@
         <v>11</v>
       </c>
       <c r="E3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F3" t="s">
         <v>13</v>
@@ -764,7 +762,9 @@
       <c r="G3" t="s">
         <v>14</v>
       </c>
-      <c r="H3"/>
+      <c r="H3" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
@@ -794,10 +794,10 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="B5" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="C5" t="s">
         <v>10</v>
@@ -806,7 +806,7 @@
         <v>11</v>
       </c>
       <c r="E5" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="F5" t="s">
         <v>13</v>
@@ -815,15 +815,15 @@
         <v>14</v>
       </c>
       <c r="H5" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>26</v>
+        <v>8</v>
       </c>
       <c r="B6" t="s">
-        <v>27</v>
+        <v>9</v>
       </c>
       <c r="C6" t="s">
         <v>10</v>
@@ -832,33 +832,31 @@
         <v>11</v>
       </c>
       <c r="E6" t="s">
-        <v>28</v>
+        <v>12</v>
       </c>
       <c r="F6" t="s">
         <v>13</v>
       </c>
       <c r="G6" t="s">
-        <v>29</v>
-      </c>
-      <c r="H6" t="s">
-        <v>30</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="H6"/>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="B7" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C7" t="s">
         <v>10</v>
       </c>
       <c r="D7" t="s">
-        <v>11</v>
+        <v>25</v>
       </c>
       <c r="E7" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="F7" t="s">
         <v>13</v>
@@ -867,15 +865,15 @@
         <v>14</v>
       </c>
       <c r="H7" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="B8" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="C8" t="s">
         <v>10</v>
@@ -884,13 +882,13 @@
         <v>11</v>
       </c>
       <c r="E8" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="F8" t="s">
         <v>13</v>
       </c>
       <c r="G8" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="H8" t="s">
         <v>22</v>
@@ -898,69 +896,71 @@
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B9" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="C9" t="s">
-        <v>38</v>
+        <v>10</v>
       </c>
       <c r="D9" t="s">
-        <v>39</v>
+        <v>11</v>
       </c>
       <c r="E9" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="F9" t="s">
-        <v>41</v>
+        <v>13</v>
       </c>
       <c r="G9" t="s">
-        <v>42</v>
+        <v>14</v>
       </c>
       <c r="H9" t="s">
-        <v>43</v>
+        <v>22</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="B10" t="s">
-        <v>17</v>
+        <v>36</v>
       </c>
       <c r="C10" t="s">
         <v>10</v>
       </c>
       <c r="D10" t="s">
-        <v>11</v>
+        <v>37</v>
       </c>
       <c r="E10" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="F10" t="s">
-        <v>13</v>
+        <v>39</v>
       </c>
       <c r="G10" t="s">
-        <v>14</v>
-      </c>
-      <c r="H10"/>
+        <v>40</v>
+      </c>
+      <c r="H10" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B11" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C11" t="s">
         <v>10</v>
       </c>
       <c r="D11" t="s">
-        <v>48</v>
+        <v>11</v>
       </c>
       <c r="E11" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="F11" t="s">
         <v>13</v>
@@ -969,41 +969,39 @@
         <v>14</v>
       </c>
       <c r="H11" t="s">
-        <v>50</v>
+        <v>22</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="B12" t="s">
-        <v>37</v>
+        <v>46</v>
       </c>
       <c r="C12" t="s">
         <v>10</v>
       </c>
       <c r="D12" t="s">
-        <v>52</v>
+        <v>11</v>
       </c>
       <c r="E12" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="F12" t="s">
-        <v>41</v>
+        <v>13</v>
       </c>
       <c r="G12" t="s">
-        <v>42</v>
-      </c>
-      <c r="H12" t="s">
-        <v>43</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="H12"/>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="B13" t="s">
-        <v>17</v>
+        <v>33</v>
       </c>
       <c r="C13" t="s">
         <v>10</v>
@@ -1012,502 +1010,604 @@
         <v>11</v>
       </c>
       <c r="E13" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="F13" t="s">
         <v>13</v>
       </c>
       <c r="G13" t="s">
-        <v>14</v>
-      </c>
-      <c r="H13"/>
+        <v>31</v>
+      </c>
+      <c r="H13" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="B14" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="C14" t="s">
-        <v>10</v>
+        <v>53</v>
       </c>
       <c r="D14" t="s">
+        <v>37</v>
+      </c>
+      <c r="E14" t="s">
+        <v>54</v>
+      </c>
+      <c r="F14" t="s">
         <v>39</v>
       </c>
-      <c r="E14" t="s">
-        <v>58</v>
-      </c>
-      <c r="F14" t="s">
+      <c r="G14" t="s">
+        <v>40</v>
+      </c>
+      <c r="H14" t="s">
         <v>41</v>
-      </c>
-      <c r="G14" t="s">
-        <v>42</v>
-      </c>
-      <c r="H14" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B15" t="s">
+        <v>56</v>
+      </c>
+      <c r="C15" t="s">
+        <v>53</v>
+      </c>
+      <c r="D15" t="s">
+        <v>11</v>
+      </c>
+      <c r="E15" t="s">
         <v>57</v>
       </c>
-      <c r="C15" t="s">
-        <v>10</v>
-      </c>
-      <c r="D15" t="s">
-        <v>39</v>
-      </c>
-      <c r="E15" t="s">
-        <v>60</v>
-      </c>
       <c r="F15" t="s">
-        <v>41</v>
+        <v>13</v>
       </c>
       <c r="G15" t="s">
-        <v>42</v>
+        <v>14</v>
       </c>
       <c r="H15" t="s">
-        <v>43</v>
+        <v>22</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B16" t="s">
-        <v>57</v>
+        <v>36</v>
       </c>
       <c r="C16" t="s">
         <v>10</v>
       </c>
       <c r="D16" t="s">
+        <v>37</v>
+      </c>
+      <c r="E16" t="s">
+        <v>59</v>
+      </c>
+      <c r="F16" t="s">
         <v>39</v>
       </c>
-      <c r="E16" t="s">
-        <v>62</v>
-      </c>
-      <c r="F16" t="s">
+      <c r="G16" t="s">
+        <v>40</v>
+      </c>
+      <c r="H16" t="s">
         <v>41</v>
-      </c>
-      <c r="G16" t="s">
-        <v>42</v>
-      </c>
-      <c r="H16" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>63</v>
+        <v>8</v>
       </c>
       <c r="B17" t="s">
-        <v>64</v>
+        <v>9</v>
       </c>
       <c r="C17" t="s">
         <v>10</v>
       </c>
       <c r="D17" t="s">
-        <v>39</v>
+        <v>11</v>
       </c>
       <c r="E17" t="s">
-        <v>65</v>
+        <v>12</v>
       </c>
       <c r="F17" t="s">
         <v>13</v>
       </c>
       <c r="G17" t="s">
-        <v>29</v>
+        <v>14</v>
       </c>
       <c r="H17"/>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="B18" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="C18" t="s">
         <v>10</v>
       </c>
       <c r="D18" t="s">
-        <v>48</v>
+        <v>25</v>
       </c>
       <c r="E18" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="F18" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="G18" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="H18" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="B19" t="s">
-        <v>67</v>
+        <v>52</v>
       </c>
       <c r="C19" t="s">
-        <v>10</v>
+        <v>53</v>
       </c>
       <c r="D19" t="s">
-        <v>11</v>
+        <v>37</v>
       </c>
       <c r="E19" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="F19" t="s">
-        <v>13</v>
+        <v>39</v>
       </c>
       <c r="G19" t="s">
-        <v>29</v>
+        <v>40</v>
       </c>
       <c r="H19" t="s">
-        <v>72</v>
+        <v>41</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>73</v>
+        <v>15</v>
       </c>
       <c r="B20" t="s">
-        <v>74</v>
+        <v>16</v>
       </c>
       <c r="C20" t="s">
         <v>10</v>
       </c>
       <c r="D20" t="s">
-        <v>39</v>
+        <v>11</v>
       </c>
       <c r="E20" t="s">
-        <v>75</v>
+        <v>17</v>
       </c>
       <c r="F20" t="s">
         <v>13</v>
       </c>
       <c r="G20" t="s">
-        <v>29</v>
+        <v>14</v>
       </c>
       <c r="H20" t="s">
-        <v>76</v>
+        <v>18</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
       <c r="B21" t="s">
-        <v>37</v>
+        <v>9</v>
       </c>
       <c r="C21" t="s">
-        <v>38</v>
+        <v>10</v>
       </c>
       <c r="D21" t="s">
-        <v>39</v>
+        <v>11</v>
       </c>
       <c r="E21" t="s">
-        <v>78</v>
+        <v>67</v>
       </c>
       <c r="F21" t="s">
-        <v>41</v>
+        <v>13</v>
       </c>
       <c r="G21" t="s">
-        <v>42</v>
-      </c>
-      <c r="H21" t="s">
-        <v>43</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="H21"/>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>79</v>
+        <v>68</v>
       </c>
       <c r="B22" t="s">
-        <v>74</v>
+        <v>61</v>
       </c>
       <c r="C22" t="s">
-        <v>10</v>
+        <v>53</v>
       </c>
       <c r="D22" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E22" t="s">
-        <v>80</v>
+        <v>69</v>
       </c>
       <c r="F22" t="s">
         <v>13</v>
       </c>
       <c r="G22" t="s">
-        <v>29</v>
+        <v>70</v>
       </c>
       <c r="H22" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
       <c r="B23" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="C23" t="s">
         <v>10</v>
       </c>
       <c r="D23" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
       <c r="E23" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="F23" t="s">
-        <v>41</v>
+        <v>13</v>
       </c>
       <c r="G23" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="H23" t="s">
-        <v>69</v>
+        <v>75</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="B24" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="C24" t="s">
         <v>10</v>
       </c>
       <c r="D24" t="s">
-        <v>39</v>
+        <v>11</v>
       </c>
       <c r="E24" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="F24" t="s">
         <v>13</v>
       </c>
       <c r="G24" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="H24" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="B25" t="s">
-        <v>87</v>
+        <v>52</v>
       </c>
       <c r="C25" t="s">
         <v>10</v>
       </c>
       <c r="D25" t="s">
-        <v>11</v>
+        <v>79</v>
       </c>
       <c r="E25" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="F25" t="s">
-        <v>13</v>
+        <v>39</v>
       </c>
       <c r="G25" t="s">
-        <v>14</v>
-      </c>
-      <c r="H25"/>
+        <v>40</v>
+      </c>
+      <c r="H25" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="B26" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C26" t="s">
         <v>10</v>
       </c>
       <c r="D26" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E26" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="F26" t="s">
         <v>13</v>
       </c>
       <c r="G26" t="s">
-        <v>29</v>
-      </c>
-      <c r="H26"/>
+        <v>31</v>
+      </c>
+      <c r="H26" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="B27" t="s">
-        <v>92</v>
+        <v>61</v>
       </c>
       <c r="C27" t="s">
-        <v>38</v>
+        <v>10</v>
       </c>
       <c r="D27" t="s">
-        <v>11</v>
+        <v>25</v>
       </c>
       <c r="E27" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="F27" t="s">
-        <v>13</v>
+        <v>39</v>
       </c>
       <c r="G27" t="s">
-        <v>14</v>
+        <v>31</v>
       </c>
       <c r="H27" t="s">
-        <v>22</v>
+        <v>63</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="B28" t="s">
-        <v>74</v>
+        <v>86</v>
       </c>
       <c r="C28" t="s">
         <v>10</v>
       </c>
       <c r="D28" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E28" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="F28" t="s">
         <v>13</v>
       </c>
       <c r="G28" t="s">
-        <v>29</v>
-      </c>
-      <c r="H28" t="s">
-        <v>96</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="H28"/>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="B29" t="s">
-        <v>67</v>
+        <v>9</v>
       </c>
       <c r="C29" t="s">
         <v>10</v>
       </c>
       <c r="D29" t="s">
-        <v>98</v>
+        <v>11</v>
       </c>
       <c r="E29" t="s">
-        <v>99</v>
+        <v>89</v>
       </c>
       <c r="F29" t="s">
-        <v>41</v>
+        <v>13</v>
       </c>
       <c r="G29" t="s">
-        <v>29</v>
-      </c>
-      <c r="H29" t="s">
-        <v>69</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="H29"/>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="B30" t="s">
-        <v>67</v>
+        <v>36</v>
       </c>
       <c r="C30" t="s">
         <v>10</v>
       </c>
       <c r="D30" t="s">
+        <v>37</v>
+      </c>
+      <c r="E30" t="s">
+        <v>91</v>
+      </c>
+      <c r="F30" t="s">
         <v>39</v>
       </c>
-      <c r="E30" t="s">
-        <v>101</v>
-      </c>
-      <c r="F30" t="s">
-        <v>13</v>
-      </c>
       <c r="G30" t="s">
-        <v>29</v>
+        <v>40</v>
       </c>
       <c r="H30" t="s">
-        <v>69</v>
+        <v>41</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="B31" t="s">
-        <v>103</v>
+        <v>73</v>
       </c>
       <c r="C31" t="s">
         <v>10</v>
       </c>
       <c r="D31" t="s">
-        <v>98</v>
+        <v>37</v>
       </c>
       <c r="E31" t="s">
-        <v>104</v>
+        <v>93</v>
       </c>
       <c r="F31" t="s">
         <v>13</v>
       </c>
       <c r="G31" t="s">
-        <v>105</v>
+        <v>31</v>
       </c>
       <c r="H31" t="s">
-        <v>106</v>
+        <v>94</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s">
+        <v>95</v>
+      </c>
+      <c r="B32" t="s">
+        <v>73</v>
+      </c>
+      <c r="C32" t="s">
+        <v>10</v>
+      </c>
+      <c r="D32" t="s">
+        <v>37</v>
+      </c>
+      <c r="E32" t="s">
+        <v>96</v>
+      </c>
+      <c r="F32" t="s">
+        <v>13</v>
+      </c>
+      <c r="G32" t="s">
+        <v>31</v>
+      </c>
+      <c r="H32" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="s">
+        <v>98</v>
+      </c>
+      <c r="B33" t="s">
+        <v>86</v>
+      </c>
+      <c r="C33" t="s">
+        <v>10</v>
+      </c>
+      <c r="D33" t="s">
+        <v>37</v>
+      </c>
+      <c r="E33" t="s">
+        <v>99</v>
+      </c>
+      <c r="F33" t="s">
+        <v>13</v>
+      </c>
+      <c r="G33" t="s">
+        <v>31</v>
+      </c>
+      <c r="H33"/>
+    </row>
+    <row r="34">
+      <c r="A34" t="s">
+        <v>100</v>
+      </c>
+      <c r="B34" t="s">
+        <v>101</v>
+      </c>
+      <c r="C34" t="s">
+        <v>10</v>
+      </c>
+      <c r="D34" t="s">
+        <v>102</v>
+      </c>
+      <c r="E34" t="s">
+        <v>103</v>
+      </c>
+      <c r="F34" t="s">
+        <v>13</v>
+      </c>
+      <c r="G34" t="s">
+        <v>104</v>
+      </c>
+      <c r="H34" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="s">
+        <v>106</v>
+      </c>
+      <c r="B35" t="s">
+        <v>61</v>
+      </c>
+      <c r="C35" t="s">
+        <v>10</v>
+      </c>
+      <c r="D35" t="s">
+        <v>102</v>
+      </c>
+      <c r="E35" t="s">
         <v>107</v>
       </c>
-      <c r="B32" t="s">
-        <v>67</v>
-      </c>
-      <c r="C32" t="s">
-        <v>38</v>
-      </c>
-      <c r="D32" t="s">
+      <c r="F35" t="s">
         <v>39</v>
       </c>
-      <c r="E32" t="s">
+      <c r="G35" t="s">
+        <v>31</v>
+      </c>
+      <c r="H35" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="s">
         <v>108</v>
       </c>
-      <c r="F32" t="s">
-        <v>13</v>
-      </c>
-      <c r="G32" t="s">
+      <c r="B36" t="s">
+        <v>61</v>
+      </c>
+      <c r="C36" t="s">
+        <v>10</v>
+      </c>
+      <c r="D36" t="s">
+        <v>37</v>
+      </c>
+      <c r="E36" t="s">
         <v>109</v>
       </c>
-      <c r="H32" t="s">
-        <v>72</v>
+      <c r="F36" t="s">
+        <v>13</v>
+      </c>
+      <c r="G36" t="s">
+        <v>31</v>
+      </c>
+      <c r="H36" t="s">
+        <v>63</v>
       </c>
     </row>
   </sheetData>

</xml_diff>